<commit_message>
anhvt tai lieu full
</commit_message>
<xml_diff>
--- a/SaleManager/Tài Liệu/Task_Sheet.xlsx
+++ b/SaleManager/Tài Liệu/Task_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New folder\PROJECTJAVA\Project\SaleManager\Tài Liệu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANHVT\Desktop\Tài Liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t xml:space="preserve">                                                                  Bảng phân công công việc</t>
   </si>
@@ -66,6 +66,27 @@
   </si>
   <si>
     <t>Vũ Thế Sang</t>
+  </si>
+  <si>
+    <t>Tạ Minh Hiển</t>
+  </si>
+  <si>
+    <t>Danh sách các hóa đơn bán hàng</t>
+  </si>
+  <si>
+    <t>Nhập hóa đơn bán hàng</t>
+  </si>
+  <si>
+    <t>Các chức năng thực hiện:Quản lý hóa đơn bán hàng, Khách hàng trả lại hàng cho NPP,Quản lý phiếu xuất kho cho nhân viên bán hàng</t>
+  </si>
+  <si>
+    <t>Danh sách các phiếu xuất kho</t>
+  </si>
+  <si>
+    <t>Thêm phiếu xuất kho</t>
+  </si>
+  <si>
+    <t>Danh sách các giao dịch trả lại hàng</t>
   </si>
   <si>
     <t>Vũ Tuấn Anh</t>
@@ -151,10 +172,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -165,6 +187,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,7 +545,7 @@
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -532,11 +557,11 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -544,7 +569,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -556,141 +581,141 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6">
+      <c r="B5" s="8"/>
+      <c r="C5" s="7">
         <v>42720</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7">
         <v>42721</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6">
+      <c r="B6" s="8"/>
+      <c r="C6" s="7">
         <v>42720</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7">
         <v>42723</v>
       </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6">
+      <c r="B7" s="8"/>
+      <c r="C7" s="7">
         <v>42721</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7">
         <v>42721</v>
       </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6">
+      <c r="B8" s="8"/>
+      <c r="C8" s="7">
         <v>42723</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7">
         <v>42724</v>
       </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6">
+      <c r="B9" s="8"/>
+      <c r="C9" s="7">
         <v>42724</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="6">
+      <c r="D9" s="8"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="7">
         <v>42725</v>
       </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6">
+      <c r="B10" s="8"/>
+      <c r="C10" s="7">
         <v>42725</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="6">
+      <c r="D10" s="8"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="7">
         <v>42726</v>
       </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6">
+      <c r="B11" s="8"/>
+      <c r="C11" s="7">
         <v>42724</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="7">
         <v>42725</v>
       </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -698,9 +723,9 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -708,10 +733,8 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -719,15 +742,12 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -737,188 +757,424 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="7"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6">
-        <v>42720</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6">
-        <v>42721</v>
-      </c>
-      <c r="H17" s="5"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="9"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6">
-        <v>42722</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6">
-        <v>42723</v>
-      </c>
-      <c r="H18" s="5"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7">
+        <v>42730</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="7">
+        <v>42731</v>
+      </c>
+      <c r="H18" s="8"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7">
+        <v>42730</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="7">
+        <v>42731</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7">
+        <v>42731</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="7">
+        <v>42731</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="7">
+        <v>42731</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="7">
+        <v>42731</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6">
+      <c r="B22" s="8"/>
+      <c r="C22" s="7">
+        <v>42732</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="7">
+        <v>42732</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7">
+        <v>42732</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="7">
+        <v>42732</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="7">
+        <v>42720</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="7">
+        <v>42721</v>
+      </c>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="7">
+        <v>42722</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="7">
+        <v>42723</v>
+      </c>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7">
         <v>42724</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6">
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="7">
         <v>42725</v>
       </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6">
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="7">
         <v>42726</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6">
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="7">
         <v>42727</v>
       </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6">
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="7">
         <v>42728</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6">
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="7">
         <v>42729</v>
       </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6">
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="7">
         <v>42730</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6">
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="7">
         <v>42731</v>
       </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6">
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="7">
         <v>42732</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6">
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="7">
         <v>42733</v>
       </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6">
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="7">
         <v>42732</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6">
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="7">
         <v>42733</v>
       </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6">
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="7">
         <v>42734</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6">
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="7">
         <v>42734</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H36" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="101">
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="A11:B11"/>
@@ -951,14 +1207,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="E17:F17"/>
@@ -967,22 +1215,11 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
     <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>